<commit_message>
deletion of billing in client side
</commit_message>
<xml_diff>
--- a/server/src/routes/billings/output.xlsx
+++ b/server/src/routes/billings/output.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>WATERMELON INC.</t>
+    <t>COMPLEX TECH</t>
   </si>
   <si>
-    <t>PANSOL, CALAMBA LAGUNA</t>
+    <t>COMPLEX, STA. ROSA, LAGUNA</t>
   </si>
   <si>
     <t>30 DAYS</t>
@@ -514,7 +514,7 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="6">
-        <v>45258.33595532407</v>
+        <v>45258.410515219904</v>
       </c>
     </row>
     <row r="10" ht="27.75" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -557,7 +557,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="13">
-        <v>45258.33601796297</v>
+        <v>45258.410617118054</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="12" t="s">
@@ -567,7 +567,7 @@
       <c r="F16" s="12"/>
       <c r="G16" s="15"/>
       <c r="H16" s="16">
-        <v>123</v>
+        <v>565</v>
       </c>
     </row>
     <row r="17" ht="9.75" customHeight="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -583,30 +583,20 @@
       <c r="H17" s="16"/>
     </row>
     <row r="18" ht="9.75" customHeight="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
-        <v>2</v>
-      </c>
-      <c r="B18" s="13">
-        <v>45258.33615878472</v>
-      </c>
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="14"/>
-      <c r="D18" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="15"/>
-      <c r="H18" s="16">
-        <v>214124124</v>
-      </c>
+      <c r="H18" s="16"/>
     </row>
     <row r="19" ht="9.75" customHeight="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14"/>
-      <c r="D19" s="12" t="s">
-        <v>5</v>
-      </c>
+      <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="15"/>

</xml_diff>

<commit_message>
fix the totalFee equals to NaN to newly created billing
</commit_message>
<xml_diff>
--- a/server/src/routes/billings/output.xlsx
+++ b/server/src/routes/billings/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>COMPLEX TECH</t>
   </si>
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>30 DAYS</t>
-  </si>
-  <si>
-    <t>000-416-781-000000</t>
   </si>
   <si>
     <t>SHIPMENT NO.: 123123234124</t>
@@ -514,7 +511,7 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="6">
-        <v>45258.410515219904</v>
+        <v>45261.84317129629</v>
       </c>
     </row>
     <row r="10" ht="27.75" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -537,9 +534,7 @@
         <v>GREENCROSS INCORPORATED</v>
       </c>
       <c r="E11" s="8"/>
-      <c r="G11" s="9" t="s">
-        <v>3</v>
-      </c>
+      <c r="G11" s="9"/>
       <c r="H11" s="9"/>
     </row>
     <row r="12" ht="18.75" customHeight="1" spans="4:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -557,17 +552,17 @@
         <v>1</v>
       </c>
       <c r="B16" s="13">
-        <v>45258.410617118054</v>
+        <v>45261.84322916667</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="15"/>
       <c r="H16" s="16">
-        <v>565</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" ht="9.75" customHeight="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -575,7 +570,7 @@
       <c r="B17" s="13"/>
       <c r="C17" s="14"/>
       <c r="D17" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>

</xml_diff>

<commit_message>
created a new view for listing all available billings for a specific client
</commit_message>
<xml_diff>
--- a/server/src/routes/billings/output.xlsx
+++ b/server/src/routes/billings/output.xlsx
@@ -511,7 +511,7 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="6">
-        <v>45261.84317129629</v>
+        <v>45262.00103009259</v>
       </c>
     </row>
     <row r="10" ht="27.75" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="13">
-        <v>45261.84322916667</v>
+        <v>45262.02083333333</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="12" t="s">
@@ -562,7 +562,7 @@
       <c r="F16" s="12"/>
       <c r="G16" s="15"/>
       <c r="H16" s="16">
-        <v>143</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" ht="9.75" customHeight="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
formatted the date of billingList and billing views
</commit_message>
<xml_diff>
--- a/server/src/routes/billings/output.xlsx
+++ b/server/src/routes/billings/output.xlsx
@@ -511,7 +511,7 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="6">
-        <v>45262.00103009259</v>
+        <v>45284.66666666667</v>
       </c>
     </row>
     <row r="10" ht="27.75" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="13">
-        <v>45262.02083333333</v>
+        <v>45262.262662037036</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="12" t="s">
@@ -562,7 +562,7 @@
       <c r="F16" s="12"/>
       <c r="G16" s="15"/>
       <c r="H16" s="16">
-        <v>213</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" ht="9.75" customHeight="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added placeholder for all inputs in internal and sub-contractor salary and deduction and addded the modal (not completed) for creating a payroll batch
</commit_message>
<xml_diff>
--- a/server/src/routes/billings/output.xlsx
+++ b/server/src/routes/billings/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>COMPLEX TECH</t>
   </si>
@@ -511,7 +511,7 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="6">
-        <v>45284.66666666667</v>
+        <v>45289.66666666667</v>
       </c>
     </row>
     <row r="10" ht="27.75" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="13">
-        <v>45262.262662037036</v>
+        <v>45265.298125</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="12" t="s">
@@ -562,7 +562,7 @@
       <c r="F16" s="12"/>
       <c r="G16" s="15"/>
       <c r="H16" s="16">
-        <v>5</v>
+        <v>500</v>
       </c>
     </row>
     <row r="17" ht="9.75" customHeight="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -578,20 +578,30 @@
       <c r="H17" s="16"/>
     </row>
     <row r="18" ht="9.75" customHeight="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
+      <c r="A18" s="12">
+        <v>2</v>
+      </c>
+      <c r="B18" s="13">
+        <v>45265.29819444445</v>
+      </c>
       <c r="C18" s="14"/>
-      <c r="D18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>3</v>
+      </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="15"/>
-      <c r="H18" s="16"/>
+      <c r="H18" s="16">
+        <v>5555</v>
+      </c>
     </row>
     <row r="19" ht="9.75" customHeight="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14"/>
-      <c r="D19" s="12"/>
+      <c r="D19" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="15"/>

</xml_diff>

<commit_message>
fix error occurence in payroll and set placeholder for inputs
</commit_message>
<xml_diff>
--- a/server/src/routes/billings/output.xlsx
+++ b/server/src/routes/billings/output.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>COMPLEX TECH</t>
+    <t>2GO LOGISTICS</t>
   </si>
   <si>
-    <t>COMPLEX, STA. ROSA, LAGUNA</t>
+    <t>BRGY. BANAY BANAY, KATAPATAN HOMES, CABUYAO LAGUNA</t>
   </si>
   <si>
     <t>30 DAYS</t>
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="13">
-        <v>45265.298125</v>
+        <v>45270.30501157408</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="12" t="s">
@@ -578,30 +578,20 @@
       <c r="H17" s="16"/>
     </row>
     <row r="18" ht="9.75" customHeight="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
-        <v>2</v>
-      </c>
-      <c r="B18" s="13">
-        <v>45265.29819444445</v>
-      </c>
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="14"/>
-      <c r="D18" s="12" t="s">
-        <v>3</v>
-      </c>
+      <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="15"/>
-      <c r="H18" s="16">
-        <v>5555</v>
-      </c>
+      <c r="H18" s="16"/>
     </row>
     <row r="19" ht="9.75" customHeight="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14"/>
-      <c r="D19" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="15"/>

</xml_diff>

<commit_message>
added placeholder for the transaction number
</commit_message>
<xml_diff>
--- a/server/src/routes/billings/output.xlsx
+++ b/server/src/routes/billings/output.xlsx
@@ -16,10 +16,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>2GO LOGISTICS</t>
+    <t>COMPLEX, STA. ROSA, LAGUNA</t>
   </si>
   <si>
-    <t>BRGY. BANAY BANAY, KATAPATAN HOMES, CABUYAO LAGUNA</t>
+    <t>COMPLEX TECH</t>
   </si>
   <si>
     <t>30 DAYS</t>
@@ -511,7 +511,7 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="6">
-        <v>45289.66666666667</v>
+        <v>45316.66666666667</v>
       </c>
     </row>
     <row r="10" ht="27.75" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="13">
-        <v>45270.30501157408</v>
+        <v>45293.8780324074</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="12" t="s">
@@ -562,7 +562,7 @@
       <c r="F16" s="12"/>
       <c r="G16" s="15"/>
       <c r="H16" s="16">
-        <v>500</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" ht="9.75" customHeight="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
removed all the data stored in the database and client's contract
</commit_message>
<xml_diff>
--- a/server/src/routes/billings/output.xlsx
+++ b/server/src/routes/billings/output.xlsx
@@ -16,10 +16,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>COMPLEX, STA. ROSA, LAGUNA</t>
+    <t>COMPLEX TECH2</t>
   </si>
   <si>
-    <t>COMPLEX TECH</t>
+    <t>COMPLEX, STA. ROSA, LAGUNA</t>
   </si>
   <si>
     <t>30 DAYS</t>
@@ -511,7 +511,7 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="6">
-        <v>45316.66666666667</v>
+        <v>45317.66666666667</v>
       </c>
     </row>
     <row r="10" ht="27.75" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="13">
-        <v>45293.8780324074</v>
+        <v>45298.25072916667</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="12" t="s">

</xml_diff>